<commit_message>
table 1 and timeline
</commit_message>
<xml_diff>
--- a/raw/timeline.xlsx
+++ b/raw/timeline.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sawyer/Documents/GitHub/wickford_cores/raw/population/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sawyer/Documents/GitHub/Balint_et_al_2024/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DDC227-9BA5-4345-B8E6-8EC93F784BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07CE3E1-B67A-EF43-AFC4-3EF9342A467F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{F60997B4-DC4C-477E-85F8-B8CB2F889D12}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F60997B4-DC4C-477E-85F8-B8CB2F889D12}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="timeline" sheetId="1" r:id="rId1"/>
+    <sheet name="population" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t>date</t>
   </si>
@@ -84,9 +85,6 @@
     <t>RI restrictions on P in detergents</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>Secondary literature</t>
   </si>
   <si>
@@ -127,6 +125,24 @@
   </si>
   <si>
     <t>Library connected to sewer</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>North Kingstown</t>
+  </si>
+  <si>
+    <t>Wickford</t>
+  </si>
+  <si>
+    <t>Census Tract 503.02</t>
   </si>
 </sst>
 </file>
@@ -478,11 +494,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A459183C-A2A8-469E-A97F-4C6FE06C7050}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -490,7 +504,7 @@
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,95 +514,74 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1703</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1710</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1727</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1728</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1795</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1815</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1875</v>
       </c>
@@ -596,27 +589,21 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1888</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1897</v>
       </c>
@@ -624,13 +611,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1899</v>
       </c>
@@ -638,13 +622,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1904</v>
       </c>
@@ -652,13 +633,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1905</v>
       </c>
@@ -666,13 +644,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1918</v>
       </c>
@@ -680,13 +655,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1930</v>
       </c>
@@ -694,41 +666,32 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1938</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1939</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1945</v>
       </c>
@@ -736,13 +699,10 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1971</v>
       </c>
@@ -750,13 +710,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1975</v>
       </c>
@@ -764,13 +721,10 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1988</v>
       </c>
@@ -778,13 +732,10 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1995</v>
       </c>
@@ -792,13 +743,10 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1998</v>
       </c>
@@ -806,38 +754,386 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2018</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2022</v>
       </c>
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B99A0A-6E73-BB47-B6EA-817D48E130D6}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1790</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>2907</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1800</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>2794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1810</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1820</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1830</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1840</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>2909</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1850</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1860</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>3104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1870</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1880</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1890</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1900</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>4194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1910</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>4048</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1920</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>3397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1930</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1940</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1950</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>14810</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1960</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>18977</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1970</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>29793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1980</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>21938</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1990</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>23786</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>26326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2010</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>26486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2020</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <v>27732</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1950</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1960</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>2934</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1990</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2000</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>2927</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2010</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2020</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>2680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>